<commit_message>
updated with epiweek, after rolling back to old version
</commit_message>
<xml_diff>
--- a/misc/designer_translations.xlsx
+++ b/misc/designer_translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\outbreak-tools\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B76A6F-E69B-4C73-BEC1-70D5521A1D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B500818F-5EB6-4AEE-87E6-095FE3D8852B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="3675" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LinelistTranslation" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2478" uniqueCount="2032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2497" uniqueCount="2045">
   <si>
     <t>Tables for translations of the linelist</t>
   </si>
@@ -6130,13 +6130,52 @@
   </si>
   <si>
     <t>Accueil</t>
+  </si>
+  <si>
+    <t>RNG_LabDefEpiWeek</t>
+  </si>
+  <si>
+    <t>يوم البدء الافتراضي لـ Epiweek</t>
+  </si>
+  <si>
+    <t>Default Epiweek start day</t>
+  </si>
+  <si>
+    <t>Jour de début d'Epiweek par défaut</t>
+  </si>
+  <si>
+    <t>Dia de início padrão da Epiweek</t>
+  </si>
+  <si>
+    <t>Día de inicio predeterminado de Epiweek</t>
+  </si>
+  <si>
+    <t>Translation of dropdowns (dropdown in the main worksheet)</t>
+  </si>
+  <si>
+    <t>DROPEPIWEEK</t>
+  </si>
+  <si>
+    <t>RNGLSTEPIWEEKENG</t>
+  </si>
+  <si>
+    <t>RNGLSTEPIWEEKARA</t>
+  </si>
+  <si>
+    <t>RNGLSTEPIWEEKPOR</t>
+  </si>
+  <si>
+    <t>RNGLSTEPIWEEKSPA</t>
+  </si>
+  <si>
+    <t>RNGLSTEPIWEEKFRA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
@@ -6162,8 +6201,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6175,8 +6225,20 @@
         <fgColor rgb="FFDCE6F1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -6195,11 +6257,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -6213,11 +6304,300 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -6309,8 +6689,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="t_tradrange" displayName="t_tradrange" ref="B76:G89" totalsRowShown="0">
-  <autoFilter ref="B76:G89" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="t_tradrange" displayName="t_tradrange" ref="B76:G90" totalsRowShown="0">
+  <autoFilter ref="B76:G90" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="MSG_ID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="ENG"/>
@@ -6333,6 +6713,21 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="SPA"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="POR"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="ARA"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBF201D7-64ED-443F-AE13-88E0A1D19EA7}" name="t_traddrop" displayName="t_traddrop" ref="B113:G114" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="B113:G114" xr:uid="{CBF201D7-64ED-443F-AE13-88E0A1D19EA7}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{017F9F65-DA3E-4D2D-A8A9-86B0311704B8}" name="MSG_ID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{8CB7068D-F258-480F-84FF-DA8083B35313}" name="ENG" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{3554A1EB-8A10-4348-B4D3-4A64A3DF6F8C}" name="FRA" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{BF9E3166-14F3-42A0-A2E7-5DBBC6154D22}" name="SPA" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{78A4B4BF-C748-49FD-A6BC-FEFC650944B9}" name="POR" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{12E1B81D-B294-471C-84A3-93485CC84B15}" name="ARA" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13084,10 +13479,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:G107"/>
+  <dimension ref="B2:G114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A99" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -14778,12 +15173,24 @@
       </c>
     </row>
     <row r="90" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
-      <c r="G90" s="2"/>
+      <c r="B90" s="2" t="s">
+        <v>2032</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>2033</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>2034</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>2036</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>2037</v>
+      </c>
     </row>
     <row r="91" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="2"/>
@@ -15091,13 +15498,59 @@
         <v>1987</v>
       </c>
     </row>
+    <row r="111" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B111" s="3" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B113" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G113" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B114" s="7" t="s">
+        <v>2039</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>2040</v>
+      </c>
+      <c r="D114" s="7" t="s">
+        <v>2044</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>2043</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>2042</v>
+      </c>
+      <c r="G114" s="7" t="s">
+        <v>2041</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed translation after test
</commit_message>
<xml_diff>
--- a/misc/designer_translations.xlsx
+++ b/misc/designer_translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\outbreak-tools\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B500818F-5EB6-4AEE-87E6-095FE3D8852B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCBFA52-0915-487F-BD37-D6142C88C192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3675" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LinelistTranslation" sheetId="1" r:id="rId1"/>
@@ -3891,9 +3891,6 @@
     <t>OptionSaturday</t>
   </si>
   <si>
-    <t>Staturday</t>
-  </si>
-  <si>
     <t>Samedi</t>
   </si>
   <si>
@@ -6169,6 +6166,9 @@
   </si>
   <si>
     <t>RNGLSTEPIWEEKFRA</t>
+  </si>
+  <si>
+    <t>Saturday</t>
   </si>
 </sst>
 </file>
@@ -6318,54 +6318,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -6579,13 +6531,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -6596,6 +6541,61 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6719,15 +6719,15 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBF201D7-64ED-443F-AE13-88E0A1D19EA7}" name="t_traddrop" displayName="t_traddrop" ref="B113:G114" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBF201D7-64ED-443F-AE13-88E0A1D19EA7}" name="t_traddrop" displayName="t_traddrop" ref="B113:G114" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B113:G114" xr:uid="{CBF201D7-64ED-443F-AE13-88E0A1D19EA7}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{017F9F65-DA3E-4D2D-A8A9-86B0311704B8}" name="MSG_ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{8CB7068D-F258-480F-84FF-DA8083B35313}" name="ENG" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{3554A1EB-8A10-4348-B4D3-4A64A3DF6F8C}" name="FRA" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{BF9E3166-14F3-42A0-A2E7-5DBBC6154D22}" name="SPA" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{78A4B4BF-C748-49FD-A6BC-FEFC650944B9}" name="POR" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{12E1B81D-B294-471C-84A3-93485CC84B15}" name="ARA" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{017F9F65-DA3E-4D2D-A8A9-86B0311704B8}" name="MSG_ID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{8CB7068D-F258-480F-84FF-DA8083B35313}" name="ENG" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{3554A1EB-8A10-4348-B4D3-4A64A3DF6F8C}" name="FRA" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{BF9E3166-14F3-42A0-A2E7-5DBBC6154D22}" name="SPA" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{78A4B4BF-C748-49FD-A6BC-FEFC650944B9}" name="POR" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{12E1B81D-B294-471C-84A3-93485CC84B15}" name="ARA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7015,8 +7015,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:G334"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A271" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C286" sqref="C286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -7320,42 +7320,42 @@
     </row>
     <row r="22" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
+        <v>2013</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>2014</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>2015</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>2016</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>2017</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>2018</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>2019</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
+        <v>2019</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>2020</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>2030</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>2023</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>2022</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>2021</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>2031</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>2024</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>2023</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>2022</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -8060,22 +8060,22 @@
     </row>
     <row r="59" spans="2:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
+        <v>2007</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>2008</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="D59" s="4" t="s">
         <v>2009</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="E59" s="4" t="s">
         <v>2010</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="F59" s="4" t="s">
         <v>2011</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="G59" s="4" t="s">
         <v>2012</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>2013</v>
       </c>
     </row>
     <row r="60" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -10414,42 +10414,42 @@
     </row>
     <row r="177" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B177" s="2" t="s">
+        <v>1991</v>
+      </c>
+      <c r="C177" s="2" t="s">
         <v>1992</v>
       </c>
-      <c r="C177" s="2" t="s">
+      <c r="D177" s="2" t="s">
+        <v>1995</v>
+      </c>
+      <c r="E177" s="2" t="s">
         <v>1993</v>
       </c>
-      <c r="D177" s="2" t="s">
+      <c r="F177" s="2" t="s">
+        <v>1994</v>
+      </c>
+      <c r="G177" s="2" t="s">
         <v>1996</v>
-      </c>
-      <c r="E177" s="2" t="s">
-        <v>1994</v>
-      </c>
-      <c r="F177" s="2" t="s">
-        <v>1995</v>
-      </c>
-      <c r="G177" s="2" t="s">
-        <v>1997</v>
       </c>
     </row>
     <row r="178" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B178" s="4" t="s">
+        <v>1997</v>
+      </c>
+      <c r="C178" s="4" t="s">
         <v>1998</v>
       </c>
-      <c r="C178" s="4" t="s">
+      <c r="D178" s="4" t="s">
+        <v>1998</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>2001</v>
+      </c>
+      <c r="F178" s="2" t="s">
         <v>1999</v>
       </c>
-      <c r="D178" s="4" t="s">
-        <v>1999</v>
-      </c>
-      <c r="E178" s="2" t="s">
-        <v>2002</v>
-      </c>
-      <c r="F178" s="2" t="s">
+      <c r="G178" s="2" t="s">
         <v>2000</v>
-      </c>
-      <c r="G178" s="2" t="s">
-        <v>2001</v>
       </c>
     </row>
     <row r="181" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -11475,19 +11475,19 @@
         <v>1108</v>
       </c>
       <c r="C233" s="4" t="s">
+        <v>1987</v>
+      </c>
+      <c r="D233" s="4" t="s">
         <v>1988</v>
       </c>
-      <c r="D233" s="4" t="s">
+      <c r="E233" s="2" t="s">
+        <v>1990</v>
+      </c>
+      <c r="F233" s="2" t="s">
+        <v>1440</v>
+      </c>
+      <c r="G233" s="2" t="s">
         <v>1989</v>
-      </c>
-      <c r="E233" s="2" t="s">
-        <v>1991</v>
-      </c>
-      <c r="F233" s="2" t="s">
-        <v>1441</v>
-      </c>
-      <c r="G233" s="2" t="s">
-        <v>1990</v>
       </c>
     </row>
     <row r="234" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -12434,220 +12434,220 @@
       <c r="B281" s="2" t="s">
         <v>1284</v>
       </c>
-      <c r="C281" s="2" t="s">
+      <c r="C281" s="4" t="s">
+        <v>2044</v>
+      </c>
+      <c r="D281" s="2" t="s">
         <v>1285</v>
       </c>
-      <c r="D281" s="2" t="s">
+      <c r="E281" s="2" t="s">
         <v>1286</v>
       </c>
-      <c r="E281" s="2" t="s">
+      <c r="F281" s="2" t="s">
+        <v>1286</v>
+      </c>
+      <c r="G281" s="2" t="s">
         <v>1287</v>
-      </c>
-      <c r="F281" s="2" t="s">
-        <v>1287</v>
-      </c>
-      <c r="G281" s="2" t="s">
-        <v>1288</v>
       </c>
     </row>
     <row r="282" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B282" s="2" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C282" s="2" t="s">
         <v>1289</v>
       </c>
-      <c r="C282" s="2" t="s">
+      <c r="D282" s="2" t="s">
         <v>1290</v>
       </c>
-      <c r="D282" s="2" t="s">
+      <c r="E282" s="2" t="s">
         <v>1291</v>
       </c>
-      <c r="E282" s="2" t="s">
+      <c r="F282" s="2" t="s">
+        <v>1291</v>
+      </c>
+      <c r="G282" s="2" t="s">
         <v>1292</v>
-      </c>
-      <c r="F282" s="2" t="s">
-        <v>1292</v>
-      </c>
-      <c r="G282" s="2" t="s">
-        <v>1293</v>
       </c>
     </row>
     <row r="283" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B283" s="2" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C283" s="2" t="s">
         <v>1294</v>
       </c>
-      <c r="C283" s="2" t="s">
+      <c r="D283" s="2" t="s">
         <v>1295</v>
       </c>
-      <c r="D283" s="2" t="s">
+      <c r="E283" s="2" t="s">
         <v>1296</v>
       </c>
-      <c r="E283" s="2" t="s">
+      <c r="F283" s="2" t="s">
         <v>1297</v>
       </c>
-      <c r="F283" s="2" t="s">
+      <c r="G283" s="2" t="s">
         <v>1298</v>
-      </c>
-      <c r="G283" s="2" t="s">
-        <v>1299</v>
       </c>
     </row>
     <row r="284" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B284" s="2" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C284" s="2" t="s">
         <v>1300</v>
       </c>
-      <c r="C284" s="2" t="s">
+      <c r="D284" s="2" t="s">
         <v>1301</v>
       </c>
-      <c r="D284" s="2" t="s">
+      <c r="E284" s="2" t="s">
         <v>1302</v>
       </c>
-      <c r="E284" s="2" t="s">
+      <c r="F284" s="2" t="s">
         <v>1303</v>
       </c>
-      <c r="F284" s="2" t="s">
+      <c r="G284" s="2" t="s">
         <v>1304</v>
-      </c>
-      <c r="G284" s="2" t="s">
-        <v>1305</v>
       </c>
     </row>
     <row r="285" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B285" s="2" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C285" s="2" t="s">
         <v>1306</v>
       </c>
-      <c r="C285" s="2" t="s">
+      <c r="D285" s="2" t="s">
         <v>1307</v>
       </c>
-      <c r="D285" s="2" t="s">
+      <c r="E285" s="2" t="s">
         <v>1308</v>
       </c>
-      <c r="E285" s="2" t="s">
+      <c r="F285" s="2" t="s">
         <v>1309</v>
       </c>
-      <c r="F285" s="2" t="s">
+      <c r="G285" s="2" t="s">
         <v>1310</v>
-      </c>
-      <c r="G285" s="2" t="s">
-        <v>1311</v>
       </c>
     </row>
     <row r="286" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B286" s="2" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C286" s="2" t="s">
         <v>1312</v>
       </c>
-      <c r="C286" s="2" t="s">
+      <c r="D286" s="2" t="s">
         <v>1313</v>
       </c>
-      <c r="D286" s="2" t="s">
+      <c r="E286" s="2" t="s">
         <v>1314</v>
       </c>
-      <c r="E286" s="2" t="s">
+      <c r="F286" s="2" t="s">
         <v>1315</v>
       </c>
-      <c r="F286" s="2" t="s">
+      <c r="G286" s="2" t="s">
         <v>1316</v>
-      </c>
-      <c r="G286" s="2" t="s">
-        <v>1317</v>
       </c>
     </row>
     <row r="287" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B287" s="2" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="C287" s="2" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D287" s="2" t="s">
         <v>1313</v>
       </c>
-      <c r="D287" s="2" t="s">
+      <c r="E287" s="2" t="s">
         <v>1314</v>
       </c>
-      <c r="E287" s="2" t="s">
+      <c r="F287" s="2" t="s">
         <v>1315</v>
       </c>
-      <c r="F287" s="2" t="s">
+      <c r="G287" s="2" t="s">
         <v>1316</v>
-      </c>
-      <c r="G287" s="2" t="s">
-        <v>1317</v>
       </c>
     </row>
     <row r="288" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B288" s="2" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C288" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="C288" s="2" t="s">
+      <c r="D288" s="2" t="s">
         <v>1320</v>
       </c>
-      <c r="D288" s="2" t="s">
+      <c r="E288" s="2" t="s">
         <v>1321</v>
       </c>
-      <c r="E288" s="2" t="s">
+      <c r="F288" s="2" t="s">
         <v>1322</v>
       </c>
-      <c r="F288" s="2" t="s">
+      <c r="G288" s="2" t="s">
         <v>1323</v>
-      </c>
-      <c r="G288" s="2" t="s">
-        <v>1324</v>
       </c>
     </row>
     <row r="289" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B289" s="2" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="C289" s="2" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D289" s="2" t="s">
         <v>1320</v>
       </c>
-      <c r="D289" s="2" t="s">
+      <c r="E289" s="2" t="s">
         <v>1321</v>
       </c>
-      <c r="E289" s="2" t="s">
+      <c r="F289" s="2" t="s">
         <v>1322</v>
       </c>
-      <c r="F289" s="2" t="s">
+      <c r="G289" s="2" t="s">
         <v>1323</v>
-      </c>
-      <c r="G289" s="2" t="s">
-        <v>1324</v>
       </c>
     </row>
     <row r="290" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B290" s="2" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C290" s="2" t="s">
         <v>1326</v>
       </c>
-      <c r="C290" s="2" t="s">
+      <c r="D290" s="2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="E290" s="2" t="s">
         <v>1327</v>
       </c>
-      <c r="D290" s="2" t="s">
-        <v>1327</v>
-      </c>
-      <c r="E290" s="2" t="s">
+      <c r="F290" s="2" t="s">
         <v>1328</v>
       </c>
-      <c r="F290" s="2" t="s">
+      <c r="G290" s="2" t="s">
         <v>1329</v>
-      </c>
-      <c r="G290" s="2" t="s">
-        <v>1330</v>
       </c>
     </row>
     <row r="291" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B291" s="2" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="C291" s="2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D291" s="2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="E291" s="2" t="s">
         <v>1327</v>
       </c>
-      <c r="D291" s="2" t="s">
-        <v>1327</v>
-      </c>
-      <c r="E291" s="2" t="s">
+      <c r="F291" s="2" t="s">
         <v>1328</v>
       </c>
-      <c r="F291" s="2" t="s">
+      <c r="G291" s="2" t="s">
         <v>1329</v>
-      </c>
-      <c r="G291" s="2" t="s">
-        <v>1330</v>
       </c>
     </row>
     <row r="292" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -12668,7 +12668,7 @@
     </row>
     <row r="294" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B294" s="3" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
@@ -12706,13 +12706,13 @@
     </row>
     <row r="297" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B297" s="2" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C297" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="E297" s="2" t="s">
         <v>65</v>
@@ -12726,13 +12726,13 @@
     </row>
     <row r="298" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B298" s="2" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C298" s="2" t="s">
         <v>1335</v>
       </c>
-      <c r="C298" s="2" t="s">
+      <c r="D298" s="2" t="s">
         <v>1336</v>
-      </c>
-      <c r="D298" s="2" t="s">
-        <v>1337</v>
       </c>
       <c r="E298" s="2" t="s">
         <v>142</v>
@@ -12746,53 +12746,53 @@
     </row>
     <row r="299" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B299" s="2" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C299" s="2" t="s">
         <v>1338</v>
       </c>
-      <c r="C299" s="2" t="s">
+      <c r="D299" s="2" t="s">
         <v>1339</v>
       </c>
-      <c r="D299" s="2" t="s">
+      <c r="E299" s="2" t="s">
         <v>1340</v>
       </c>
-      <c r="E299" s="2" t="s">
+      <c r="F299" s="2" t="s">
         <v>1341</v>
       </c>
-      <c r="F299" s="2" t="s">
+      <c r="G299" s="2" t="s">
         <v>1342</v>
-      </c>
-      <c r="G299" s="2" t="s">
-        <v>1343</v>
       </c>
     </row>
     <row r="300" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B300" s="2" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C300" s="2" t="s">
         <v>1344</v>
-      </c>
-      <c r="C300" s="2" t="s">
-        <v>1345</v>
       </c>
       <c r="D300" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E300" s="2" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="F300" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G300" s="2" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="301" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B301" s="2" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="C301" s="2" t="s">
         <v>1103</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="E301" s="2" t="s">
         <v>1105</v>
@@ -12801,98 +12801,98 @@
         <v>1106</v>
       </c>
       <c r="G301" s="2" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="302" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B302" s="2" t="s">
+        <v>1350</v>
+      </c>
+      <c r="C302" s="2" t="s">
         <v>1351</v>
       </c>
-      <c r="C302" s="2" t="s">
+      <c r="D302" s="2" t="s">
         <v>1352</v>
       </c>
-      <c r="D302" s="2" t="s">
+      <c r="E302" s="2" t="s">
         <v>1353</v>
       </c>
-      <c r="E302" s="2" t="s">
+      <c r="F302" s="2" t="s">
         <v>1354</v>
       </c>
-      <c r="F302" s="2" t="s">
+      <c r="G302" s="2" t="s">
         <v>1355</v>
-      </c>
-      <c r="G302" s="2" t="s">
-        <v>1356</v>
       </c>
     </row>
     <row r="303" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B303" s="2" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C303" s="2" t="s">
         <v>1357</v>
       </c>
-      <c r="C303" s="2" t="s">
+      <c r="D303" s="2" t="s">
         <v>1358</v>
       </c>
-      <c r="D303" s="2" t="s">
+      <c r="E303" s="2" t="s">
         <v>1359</v>
       </c>
-      <c r="E303" s="2" t="s">
+      <c r="F303" s="2" t="s">
         <v>1360</v>
       </c>
-      <c r="F303" s="2" t="s">
+      <c r="G303" s="2" t="s">
         <v>1361</v>
-      </c>
-      <c r="G303" s="2" t="s">
-        <v>1362</v>
       </c>
     </row>
     <row r="304" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B304" s="2" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C304" s="2" t="s">
         <v>1363</v>
       </c>
-      <c r="C304" s="2" t="s">
+      <c r="D304" s="2" t="s">
         <v>1364</v>
       </c>
-      <c r="D304" s="2" t="s">
+      <c r="E304" s="2" t="s">
         <v>1365</v>
       </c>
-      <c r="E304" s="2" t="s">
+      <c r="F304" s="2" t="s">
         <v>1366</v>
       </c>
-      <c r="F304" s="2" t="s">
+      <c r="G304" s="2" t="s">
         <v>1367</v>
-      </c>
-      <c r="G304" s="2" t="s">
-        <v>1368</v>
       </c>
     </row>
     <row r="305" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B305" s="2" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="C305" s="4" t="s">
+        <v>2002</v>
+      </c>
+      <c r="D305" s="4" t="s">
+        <v>2004</v>
+      </c>
+      <c r="E305" s="4" t="s">
         <v>2003</v>
       </c>
-      <c r="D305" s="4" t="s">
+      <c r="F305" s="4" t="s">
         <v>2005</v>
       </c>
-      <c r="E305" s="4" t="s">
-        <v>2004</v>
-      </c>
-      <c r="F305" s="4" t="s">
+      <c r="G305" s="4" t="s">
         <v>2006</v>
-      </c>
-      <c r="G305" s="4" t="s">
-        <v>2007</v>
       </c>
     </row>
     <row r="306" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B306" s="2" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C306" s="2" t="s">
         <v>1370</v>
       </c>
-      <c r="C306" s="2" t="s">
+      <c r="D306" s="2" t="s">
         <v>1371</v>
-      </c>
-      <c r="D306" s="2" t="s">
-        <v>1372</v>
       </c>
       <c r="E306" s="2" t="s">
         <v>1117</v>
@@ -12906,67 +12906,67 @@
     </row>
     <row r="307" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B307" s="2" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C307" s="2" t="s">
         <v>1373</v>
       </c>
-      <c r="C307" s="2" t="s">
+      <c r="D307" s="2" t="s">
         <v>1374</v>
       </c>
-      <c r="D307" s="2" t="s">
+      <c r="E307" s="2" t="s">
         <v>1375</v>
       </c>
-      <c r="E307" s="2" t="s">
+      <c r="F307" s="2" t="s">
+        <v>1375</v>
+      </c>
+      <c r="G307" s="2" t="s">
         <v>1376</v>
-      </c>
-      <c r="F307" s="2" t="s">
-        <v>1376</v>
-      </c>
-      <c r="G307" s="2" t="s">
-        <v>1377</v>
       </c>
     </row>
     <row r="308" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B308" s="2" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C308" s="2" t="s">
         <v>1378</v>
       </c>
-      <c r="C308" s="2" t="s">
+      <c r="D308" s="2" t="s">
         <v>1379</v>
       </c>
-      <c r="D308" s="2" t="s">
+      <c r="E308" s="2" t="s">
         <v>1380</v>
       </c>
-      <c r="E308" s="2" t="s">
+      <c r="F308" s="2" t="s">
         <v>1381</v>
       </c>
-      <c r="F308" s="2" t="s">
+      <c r="G308" s="2" t="s">
         <v>1382</v>
-      </c>
-      <c r="G308" s="2" t="s">
-        <v>1383</v>
       </c>
     </row>
     <row r="309" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B309" s="2" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C309" s="2" t="s">
         <v>1384</v>
       </c>
-      <c r="C309" s="2" t="s">
+      <c r="D309" s="2" t="s">
         <v>1385</v>
       </c>
-      <c r="D309" s="2" t="s">
+      <c r="E309" s="2" t="s">
         <v>1386</v>
       </c>
-      <c r="E309" s="2" t="s">
+      <c r="F309" s="2" t="s">
         <v>1387</v>
       </c>
-      <c r="F309" s="2" t="s">
+      <c r="G309" s="2" t="s">
         <v>1388</v>
-      </c>
-      <c r="G309" s="2" t="s">
-        <v>1389</v>
       </c>
     </row>
     <row r="310" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B310" s="2" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="C310" s="2" t="s">
         <v>43</v>
@@ -12986,7 +12986,7 @@
     </row>
     <row r="311" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B311" s="2" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="C311" s="2" t="s">
         <v>1015</v>
@@ -13006,13 +13006,13 @@
     </row>
     <row r="312" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B312" s="2" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C312" s="2" t="s">
         <v>1021</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="E312" s="2" t="s">
         <v>1023</v>
@@ -13021,72 +13021,72 @@
         <v>1023</v>
       </c>
       <c r="G312" s="2" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="313" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B313" s="2" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C313" s="2" t="s">
         <v>1395</v>
       </c>
-      <c r="C313" s="2" t="s">
+      <c r="D313" s="2" t="s">
         <v>1396</v>
       </c>
-      <c r="D313" s="2" t="s">
+      <c r="E313" s="2" t="s">
         <v>1397</v>
       </c>
-      <c r="E313" s="2" t="s">
+      <c r="F313" s="2" t="s">
+        <v>1397</v>
+      </c>
+      <c r="G313" s="2" t="s">
         <v>1398</v>
-      </c>
-      <c r="F313" s="2" t="s">
-        <v>1398</v>
-      </c>
-      <c r="G313" s="2" t="s">
-        <v>1399</v>
       </c>
     </row>
     <row r="314" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B314" s="2" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C314" s="2" t="s">
         <v>1400</v>
       </c>
-      <c r="C314" s="2" t="s">
+      <c r="D314" s="2" t="s">
         <v>1401</v>
       </c>
-      <c r="D314" s="2" t="s">
+      <c r="E314" s="2" t="s">
         <v>1402</v>
       </c>
-      <c r="E314" s="2" t="s">
+      <c r="F314" s="2" t="s">
         <v>1403</v>
       </c>
-      <c r="F314" s="2" t="s">
+      <c r="G314" s="2" t="s">
         <v>1404</v>
-      </c>
-      <c r="G314" s="2" t="s">
-        <v>1405</v>
       </c>
     </row>
     <row r="315" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B315" s="2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C315" s="2" t="s">
         <v>1406</v>
       </c>
-      <c r="C315" s="2" t="s">
+      <c r="D315" s="2" t="s">
         <v>1407</v>
       </c>
-      <c r="D315" s="2" t="s">
+      <c r="E315" s="2" t="s">
         <v>1408</v>
       </c>
-      <c r="E315" s="2" t="s">
+      <c r="F315" s="2" t="s">
         <v>1409</v>
       </c>
-      <c r="F315" s="2" t="s">
+      <c r="G315" s="2" t="s">
         <v>1410</v>
-      </c>
-      <c r="G315" s="2" t="s">
-        <v>1411</v>
       </c>
     </row>
     <row r="316" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B316" s="2" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="C316" s="2" t="s">
         <v>46</v>
@@ -13106,127 +13106,127 @@
     </row>
     <row r="317" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B317" s="2" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C317" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="C317" s="2" t="s">
+      <c r="D317" s="2" t="s">
         <v>1414</v>
       </c>
-      <c r="D317" s="2" t="s">
+      <c r="E317" s="2" t="s">
         <v>1415</v>
       </c>
-      <c r="E317" s="2" t="s">
+      <c r="F317" s="2" t="s">
         <v>1416</v>
       </c>
-      <c r="F317" s="2" t="s">
+      <c r="G317" s="2" t="s">
         <v>1417</v>
-      </c>
-      <c r="G317" s="2" t="s">
-        <v>1418</v>
       </c>
     </row>
     <row r="318" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B318" s="2" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C318" s="2" t="s">
         <v>1419</v>
       </c>
-      <c r="C318" s="2" t="s">
+      <c r="D318" s="2" t="s">
         <v>1420</v>
       </c>
-      <c r="D318" s="2" t="s">
+      <c r="E318" s="2" t="s">
         <v>1421</v>
       </c>
-      <c r="E318" s="2" t="s">
+      <c r="F318" s="2" t="s">
         <v>1422</v>
       </c>
-      <c r="F318" s="2" t="s">
+      <c r="G318" s="2" t="s">
         <v>1423</v>
-      </c>
-      <c r="G318" s="2" t="s">
-        <v>1424</v>
       </c>
     </row>
     <row r="319" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B319" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C319" s="2" t="s">
         <v>1425</v>
       </c>
-      <c r="C319" s="2" t="s">
+      <c r="D319" s="2" t="s">
         <v>1426</v>
       </c>
-      <c r="D319" s="2" t="s">
+      <c r="E319" s="2" t="s">
         <v>1427</v>
       </c>
-      <c r="E319" s="2" t="s">
+      <c r="F319" s="2" t="s">
         <v>1428</v>
       </c>
-      <c r="F319" s="2" t="s">
+      <c r="G319" s="2" t="s">
         <v>1429</v>
-      </c>
-      <c r="G319" s="2" t="s">
-        <v>1430</v>
       </c>
     </row>
     <row r="320" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B320" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C320" s="2" t="s">
         <v>1431</v>
       </c>
-      <c r="C320" s="2" t="s">
+      <c r="D320" s="2" t="s">
         <v>1432</v>
       </c>
-      <c r="D320" s="2" t="s">
+      <c r="E320" s="2" t="s">
         <v>1433</v>
       </c>
-      <c r="E320" s="2" t="s">
+      <c r="F320" s="2" t="s">
         <v>1434</v>
       </c>
-      <c r="F320" s="2" t="s">
+      <c r="G320" s="2" t="s">
         <v>1435</v>
-      </c>
-      <c r="G320" s="2" t="s">
-        <v>1436</v>
       </c>
     </row>
     <row r="321" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B321" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C321" s="2" t="s">
         <v>1437</v>
       </c>
-      <c r="C321" s="2" t="s">
+      <c r="D321" s="2" t="s">
         <v>1438</v>
       </c>
-      <c r="D321" s="2" t="s">
+      <c r="E321" s="2" t="s">
         <v>1439</v>
       </c>
-      <c r="E321" s="2" t="s">
+      <c r="F321" s="2" t="s">
         <v>1440</v>
       </c>
-      <c r="F321" s="2" t="s">
+      <c r="G321" s="2" t="s">
         <v>1441</v>
-      </c>
-      <c r="G321" s="2" t="s">
-        <v>1442</v>
       </c>
     </row>
     <row r="322" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B322" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C322" s="2" t="s">
         <v>1443</v>
       </c>
-      <c r="C322" s="2" t="s">
+      <c r="D322" s="2" t="s">
         <v>1444</v>
       </c>
-      <c r="D322" s="2" t="s">
+      <c r="E322" s="2" t="s">
         <v>1445</v>
       </c>
-      <c r="E322" s="2" t="s">
+      <c r="F322" s="2" t="s">
         <v>1446</v>
       </c>
-      <c r="F322" s="2" t="s">
+      <c r="G322" s="2" t="s">
         <v>1447</v>
-      </c>
-      <c r="G322" s="2" t="s">
-        <v>1448</v>
       </c>
     </row>
     <row r="323" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B323" s="2" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="C323" s="2" t="s">
         <v>1127</v>
@@ -13235,44 +13235,44 @@
         <v>1128</v>
       </c>
       <c r="E323" s="2" t="s">
+        <v>1449</v>
+      </c>
+      <c r="F323" s="2" t="s">
         <v>1450</v>
       </c>
-      <c r="F323" s="2" t="s">
+      <c r="G323" s="2" t="s">
         <v>1451</v>
-      </c>
-      <c r="G323" s="2" t="s">
-        <v>1452</v>
       </c>
     </row>
     <row r="324" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B324" s="2" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C324" s="2" t="s">
         <v>1453</v>
       </c>
-      <c r="C324" s="2" t="s">
+      <c r="D324" s="2" t="s">
         <v>1454</v>
       </c>
-      <c r="D324" s="2" t="s">
+      <c r="E324" s="2" t="s">
         <v>1455</v>
       </c>
-      <c r="E324" s="2" t="s">
+      <c r="F324" s="2" t="s">
         <v>1456</v>
       </c>
-      <c r="F324" s="2" t="s">
+      <c r="G324" s="2" t="s">
         <v>1457</v>
-      </c>
-      <c r="G324" s="2" t="s">
-        <v>1458</v>
       </c>
     </row>
     <row r="325" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B325" s="2" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="C325" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D325" s="2" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="E325" s="2" t="s">
         <v>65</v>
@@ -13286,7 +13286,7 @@
     </row>
     <row r="326" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B326" s="2" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="C326" s="2" t="s">
         <v>141</v>
@@ -13306,7 +13306,7 @@
     </row>
     <row r="327" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B327" s="2" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="C327" s="2" t="s">
         <v>1110</v>
@@ -13326,13 +13326,13 @@
     </row>
     <row r="328" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B328" s="2" t="s">
+        <v>1461</v>
+      </c>
+      <c r="C328" s="2" t="s">
         <v>1462</v>
       </c>
-      <c r="C328" s="2" t="s">
-        <v>1463</v>
-      </c>
       <c r="D328" s="2" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="E328" s="2" t="s">
         <v>531</v>
@@ -13346,27 +13346,27 @@
     </row>
     <row r="329" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B329" s="2" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C329" s="2" t="s">
         <v>1464</v>
       </c>
-      <c r="C329" s="2" t="s">
+      <c r="D329" s="2" t="s">
         <v>1465</v>
       </c>
-      <c r="D329" s="2" t="s">
+      <c r="E329" s="2" t="s">
         <v>1466</v>
       </c>
-      <c r="E329" s="2" t="s">
+      <c r="F329" s="2" t="s">
         <v>1467</v>
       </c>
-      <c r="F329" s="2" t="s">
+      <c r="G329" s="2" t="s">
         <v>1468</v>
-      </c>
-      <c r="G329" s="2" t="s">
-        <v>1469</v>
       </c>
     </row>
     <row r="330" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B330" s="2" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="C330" s="2" t="s">
         <v>43</v>
@@ -13386,47 +13386,47 @@
     </row>
     <row r="331" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B331" s="2" t="s">
+        <v>1470</v>
+      </c>
+      <c r="C331" s="2" t="s">
         <v>1471</v>
       </c>
-      <c r="C331" s="2" t="s">
+      <c r="D331" s="2" t="s">
         <v>1472</v>
       </c>
-      <c r="D331" s="2" t="s">
+      <c r="E331" s="2" t="s">
         <v>1473</v>
       </c>
-      <c r="E331" s="2" t="s">
+      <c r="F331" s="2" t="s">
         <v>1474</v>
       </c>
-      <c r="F331" s="2" t="s">
+      <c r="G331" s="2" t="s">
         <v>1475</v>
-      </c>
-      <c r="G331" s="2" t="s">
-        <v>1476</v>
       </c>
     </row>
     <row r="332" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B332" s="2" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C332" s="2" t="s">
         <v>1477</v>
       </c>
-      <c r="C332" s="2" t="s">
+      <c r="D332" s="2" t="s">
         <v>1478</v>
       </c>
-      <c r="D332" s="2" t="s">
+      <c r="E332" s="2" t="s">
         <v>1479</v>
       </c>
-      <c r="E332" s="2" t="s">
+      <c r="F332" s="2" t="s">
+        <v>1479</v>
+      </c>
+      <c r="G332" s="2" t="s">
         <v>1480</v>
-      </c>
-      <c r="F332" s="2" t="s">
-        <v>1480</v>
-      </c>
-      <c r="G332" s="2" t="s">
-        <v>1481</v>
       </c>
     </row>
     <row r="333" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B333" s="2" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="C333" s="2" t="s">
         <v>80</v>
@@ -13441,27 +13441,27 @@
         <v>83</v>
       </c>
       <c r="G333" s="2" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="334" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B334" s="2" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C334" s="2" t="s">
         <v>1484</v>
       </c>
-      <c r="C334" s="2" t="s">
+      <c r="D334" s="2" t="s">
         <v>1485</v>
       </c>
-      <c r="D334" s="2" t="s">
+      <c r="E334" s="2" t="s">
         <v>1486</v>
       </c>
-      <c r="E334" s="2" t="s">
+      <c r="F334" s="2" t="s">
         <v>1487</v>
       </c>
-      <c r="F334" s="2" t="s">
+      <c r="G334" s="2" t="s">
         <v>1488</v>
-      </c>
-      <c r="G334" s="2" t="s">
-        <v>1489</v>
       </c>
     </row>
   </sheetData>
@@ -13481,8 +13481,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:G114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A99" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -13510,7 +13510,7 @@
     </row>
     <row r="4" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -13548,13 +13548,13 @@
     </row>
     <row r="7" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1103</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>1105</v>
@@ -13568,342 +13568,342 @@
     </row>
     <row r="8" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>1580</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>1581</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>1582</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>1583</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>1584</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>1585</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
+        <v>1781</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>1782</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>1783</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>1784</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>1785</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>1786</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>1787</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>1599</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>1600</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>1601</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>1602</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>1603</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>1604</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>1496</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>1497</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>1498</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>1499</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>1500</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>1501</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>1537</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>1538</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>1539</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>1540</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>1541</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>1542</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
+        <v>1639</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>1640</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>1641</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>1642</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
+        <v>1642</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>1643</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>1643</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>1644</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
+        <v>1654</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>1655</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>1656</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>1657</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>1658</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>1659</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>1660</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
+        <v>1775</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>1776</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>1777</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>1778</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>1779</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>1780</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>1781</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
+        <v>1665</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>1666</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>1667</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>1668</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>1669</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>1670</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>1628</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>1629</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>1630</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>1631</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>1632</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>1633</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
+        <v>1787</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>1788</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>1789</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>1790</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
+        <v>1790</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>1791</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>1791</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>1792</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>1793</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>1794</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>1795</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>1796</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>1797</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>1798</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>1520</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>1521</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>1522</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>1523</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>1524</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>1525</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>1502</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>1503</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>1504</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>1505</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>1506</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>1507</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
+        <v>1741</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>1742</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>1743</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>1744</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>1745</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>1491</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>1492</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>1493</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>1494</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>1495</v>
-      </c>
       <c r="G23" s="2" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
+        <v>1682</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>1683</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>1684</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>1685</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>1686</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>1687</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>1688</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -13914,7 +13914,7 @@
         <v>275</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>277</v>
@@ -13923,18 +13923,18 @@
         <v>278</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>275</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>277</v>
@@ -13943,47 +13943,47 @@
         <v>278</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
+        <v>1568</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>1569</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>1570</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>1571</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>1572</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>1573</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>1574</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>1549</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>1550</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>1551</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>1552</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>1553</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>1554</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -13991,64 +13991,64 @@
         <v>399</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>1574</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>1575</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>1576</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>1577</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>1578</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>1579</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>1730</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>1731</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>1733</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>1734</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>1735</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
+        <v>1585</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>1586</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>1587</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>1588</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>1589</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>1590</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>1591</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>43</v>
@@ -14068,133 +14068,133 @@
     </row>
     <row r="33" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
+        <v>1763</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>1764</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>1765</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>1766</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>1767</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>1768</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>1769</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>1822</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>1823</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>1824</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>1825</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>1826</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>1827</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
+        <v>1798</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>1799</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>1800</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>1802</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>1803</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>1804</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>1805</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>1806</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>1807</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
+        <v>1807</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>1808</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>1808</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>1809</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>1816</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>1817</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>1818</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>1819</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>1820</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>1821</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>1701</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>1702</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>1703</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>1704</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>1705</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>1706</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>531</v>
@@ -14203,227 +14203,227 @@
         <v>532</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
+        <v>2024</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>2027</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>2025</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="E40" s="4" t="s">
+        <v>2026</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>2028</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>2026</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>2027</v>
-      </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>2029</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>2030</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>1837</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>1838</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>1839</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>1840</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>1841</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>1842</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>1514</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>1515</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>1516</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>1517</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>1518</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>1519</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
+        <v>1830</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>1831</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>1832</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>1833</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>1834</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>1835</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>1836</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
+        <v>1621</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>1622</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>1623</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>1624</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>1625</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>1626</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>1627</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
+        <v>1649</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>1650</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>1651</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>1652</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>1653</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>1654</v>
-      </c>
       <c r="G45" s="2" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
+        <v>1809</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>1810</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>1811</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>1812</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>1813</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="G46" s="2" t="s">
         <v>1814</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>1815</v>
       </c>
     </row>
     <row r="47" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
+        <v>1644</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>1645</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>1646</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>1647</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>1648</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>1649</v>
-      </c>
       <c r="G47" s="2" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>1737</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>1738</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>1739</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>1740</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>1741</v>
-      </c>
       <c r="G48" s="2" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="49" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>1746</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>1747</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>1748</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>1749</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>1750</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>1751</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
+        <v>1615</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>1616</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>1617</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>1618</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>1619</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>1620</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>1621</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -14431,439 +14431,439 @@
         <v>558</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>1610</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>1611</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>1612</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>1613</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>1614</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>1615</v>
       </c>
     </row>
     <row r="52" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>1508</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>1509</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>1510</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>1511</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>1512</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>1513</v>
       </c>
     </row>
     <row r="53" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>1526</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>1527</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>1528</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>1529</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>1530</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>1531</v>
       </c>
     </row>
     <row r="54" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>1671</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>1672</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>1673</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>1674</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>1675</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>1676</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>1563</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>1564</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>1565</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>1566</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>1567</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>1568</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
+        <v>1676</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>1677</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>1678</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>1679</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="F56" s="2" t="s">
         <v>1680</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="G56" s="2" t="s">
         <v>1681</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>1682</v>
       </c>
     </row>
     <row r="57" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>1689</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>1690</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>1691</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>1692</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="G57" s="2" t="s">
         <v>1693</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>1694</v>
       </c>
     </row>
     <row r="58" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
+        <v>1694</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>1695</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>1696</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>1697</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="G58" s="2" t="s">
         <v>1699</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>1700</v>
       </c>
     </row>
     <row r="59" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
+        <v>1706</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>1707</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>1708</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>1709</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>1710</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="G59" s="2" t="s">
         <v>1711</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>1712</v>
       </c>
     </row>
     <row r="60" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>1713</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>1714</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>1715</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>1716</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="G60" s="2" t="s">
         <v>1717</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>1718</v>
       </c>
     </row>
     <row r="61" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>1719</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>1720</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>1721</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>1722</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="G61" s="2" t="s">
         <v>1723</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>1724</v>
       </c>
     </row>
     <row r="62" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>1543</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>1544</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>1545</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="F62" s="2" t="s">
         <v>1546</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="G62" s="2" t="s">
         <v>1547</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>1548</v>
       </c>
     </row>
     <row r="63" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
+        <v>1592</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>1593</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>1594</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>1595</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>1596</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="G63" s="2" t="s">
         <v>1597</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>1598</v>
       </c>
     </row>
     <row r="64" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>1532</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>1533</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>1534</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="F64" s="2" t="s">
         <v>1535</v>
       </c>
-      <c r="F64" s="2" t="s">
-        <v>1536</v>
-      </c>
       <c r="G64" s="2" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="65" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
+        <v>1604</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>1605</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>1606</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>1607</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>1608</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>1609</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>1610</v>
       </c>
     </row>
     <row r="66" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>1725</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>1726</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>1727</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>1728</v>
       </c>
-      <c r="F66" s="2" t="s">
-        <v>1729</v>
-      </c>
       <c r="G66" s="2" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="67" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="2" t="s">
+        <v>1660</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>1661</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>1662</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>1663</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>1664</v>
       </c>
-      <c r="F67" s="2" t="s">
-        <v>1665</v>
-      </c>
       <c r="G67" s="2" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="68" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="2" t="s">
+        <v>1751</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>1752</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>1753</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="E68" s="2" t="s">
         <v>1754</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="F68" s="2" t="s">
         <v>1755</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>1756</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>1757</v>
       </c>
     </row>
     <row r="69" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="2" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>1758</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>1759</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="E69" s="2" t="s">
         <v>1760</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>1761</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>1762</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>1763</v>
       </c>
     </row>
     <row r="70" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="2" t="s">
+        <v>1633</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>1634</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>1635</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>1636</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="F70" s="2" t="s">
         <v>1637</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="G70" s="2" t="s">
         <v>1638</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>1639</v>
       </c>
     </row>
     <row r="71" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="2" t="s">
+        <v>1554</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>1555</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>1556</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>1557</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>1558</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>1559</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>1560</v>
       </c>
     </row>
     <row r="72" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="2" t="s">
+        <v>1769</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>1770</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>1771</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="E72" s="2" t="s">
         <v>1772</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="F72" s="2" t="s">
         <v>1773</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="G72" s="2" t="s">
         <v>1774</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>1775</v>
       </c>
     </row>
     <row r="73" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -14876,7 +14876,7 @@
     </row>
     <row r="74" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="3" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
@@ -14914,282 +14914,282 @@
     </row>
     <row r="77" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="2" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>1844</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>1845</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="E77" s="2" t="s">
         <v>1846</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="F77" s="2" t="s">
         <v>1847</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="G77" s="2" t="s">
         <v>1848</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>1849</v>
       </c>
     </row>
     <row r="78" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="2" t="s">
+        <v>1849</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>1850</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="D78" s="2" t="s">
+        <v>1850</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>1851</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>1851</v>
-      </c>
-      <c r="E78" s="2" t="s">
+      <c r="F78" s="2" t="s">
         <v>1852</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>1853</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>1854</v>
       </c>
     </row>
     <row r="79" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="2" t="s">
+        <v>1854</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>1855</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>1856</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>1857</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>1858</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>1859</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>1860</v>
       </c>
     </row>
     <row r="80" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="2" t="s">
+        <v>1860</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>1861</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>1862</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>1863</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>1864</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="G80" s="2" t="s">
         <v>1865</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>1866</v>
       </c>
     </row>
     <row r="81" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="2" t="s">
+        <v>1866</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>1867</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>1868</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="E81" s="2" t="s">
         <v>1869</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="F81" s="2" t="s">
         <v>1870</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="G81" s="2" t="s">
         <v>1871</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>1872</v>
       </c>
     </row>
     <row r="82" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="2" t="s">
+        <v>1872</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>1873</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>1874</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="E82" s="2" t="s">
         <v>1875</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="F82" s="2" t="s">
         <v>1876</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="G82" s="2" t="s">
         <v>1877</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>1878</v>
       </c>
     </row>
     <row r="83" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="2" t="s">
+        <v>1878</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>1879</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>1880</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="E83" s="2" t="s">
         <v>1881</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="F83" s="2" t="s">
         <v>1882</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="G83" s="2" t="s">
         <v>1883</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>1884</v>
       </c>
     </row>
     <row r="84" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="2" t="s">
+        <v>1884</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>1885</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>1886</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="E84" s="2" t="s">
         <v>1887</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>1888</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="G84" s="2" t="s">
         <v>1889</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>1890</v>
       </c>
     </row>
     <row r="85" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B85" s="2" t="s">
+        <v>1890</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>1891</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>1892</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="E85" s="2" t="s">
         <v>1893</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="F85" s="2" t="s">
         <v>1894</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="G85" s="2" t="s">
         <v>1895</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>1896</v>
       </c>
     </row>
     <row r="86" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="2" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>1837</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>1897</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>1838</v>
-      </c>
-      <c r="D86" s="2" t="s">
+      <c r="E86" s="2" t="s">
         <v>1898</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="F86" s="2" t="s">
         <v>1899</v>
       </c>
-      <c r="F86" s="2" t="s">
-        <v>1900</v>
-      </c>
       <c r="G86" s="2" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="87" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="2" t="s">
+        <v>1900</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>1901</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="D87" s="2" t="s">
         <v>1902</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="E87" s="2" t="s">
         <v>1903</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="F87" s="2" t="s">
         <v>1904</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="G87" s="2" t="s">
         <v>1905</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>1906</v>
       </c>
     </row>
     <row r="88" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="2" t="s">
+        <v>1906</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>1907</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="D88" s="2" t="s">
         <v>1908</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="E88" s="2" t="s">
         <v>1909</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="F88" s="2" t="s">
         <v>1910</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="G88" s="2" t="s">
         <v>1911</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>1912</v>
       </c>
     </row>
     <row r="89" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B89" s="2" t="s">
+        <v>1912</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>1913</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="D89" s="2" t="s">
         <v>1914</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="E89" s="2" t="s">
         <v>1915</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="F89" s="2" t="s">
+        <v>1915</v>
+      </c>
+      <c r="G89" s="2" t="s">
         <v>1916</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>1916</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>1917</v>
       </c>
     </row>
     <row r="90" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="2" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>2032</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="D90" s="2" t="s">
         <v>2033</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="E90" s="2" t="s">
         <v>2034</v>
       </c>
-      <c r="E90" s="2" t="s">
+      <c r="F90" s="2" t="s">
         <v>2035</v>
       </c>
-      <c r="F90" s="2" t="s">
+      <c r="G90" s="2" t="s">
         <v>2036</v>
-      </c>
-      <c r="G90" s="2" t="s">
-        <v>2037</v>
       </c>
     </row>
     <row r="91" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -15202,7 +15202,7 @@
     </row>
     <row r="92" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="3" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
@@ -15240,7 +15240,7 @@
     </row>
     <row r="95" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="2" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>1077</v>
@@ -15260,122 +15260,122 @@
     </row>
     <row r="96" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B96" s="2" t="s">
+        <v>1919</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>1920</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="D96" s="2" t="s">
         <v>1921</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="E96" s="2" t="s">
         <v>1922</v>
       </c>
-      <c r="E96" s="2" t="s">
+      <c r="F96" s="2" t="s">
         <v>1923</v>
       </c>
-      <c r="F96" s="2" t="s">
+      <c r="G96" s="2" t="s">
         <v>1924</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>1925</v>
       </c>
     </row>
     <row r="97" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="2" t="s">
+        <v>1925</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>1926</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="D97" s="2" t="s">
         <v>1927</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="E97" s="2" t="s">
         <v>1928</v>
       </c>
-      <c r="E97" s="2" t="s">
+      <c r="F97" s="2" t="s">
         <v>1929</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="G97" s="2" t="s">
         <v>1930</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>1931</v>
       </c>
     </row>
     <row r="98" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="2" t="s">
+        <v>1931</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>1932</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="D98" s="2" t="s">
         <v>1933</v>
       </c>
-      <c r="D98" s="2" t="s">
+      <c r="E98" s="2" t="s">
         <v>1934</v>
       </c>
-      <c r="E98" s="2" t="s">
+      <c r="F98" s="2" t="s">
         <v>1935</v>
       </c>
-      <c r="F98" s="2" t="s">
+      <c r="G98" s="2" t="s">
         <v>1936</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>1937</v>
       </c>
     </row>
     <row r="99" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="2" t="s">
+        <v>1937</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>1938</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="D99" s="2" t="s">
         <v>1939</v>
       </c>
-      <c r="D99" s="2" t="s">
+      <c r="E99" s="2" t="s">
         <v>1940</v>
       </c>
-      <c r="E99" s="2" t="s">
+      <c r="F99" s="2" t="s">
         <v>1941</v>
       </c>
-      <c r="F99" s="2" t="s">
+      <c r="G99" s="2" t="s">
         <v>1942</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>1943</v>
       </c>
     </row>
     <row r="100" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="2" t="s">
+        <v>1943</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>1944</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="D100" s="2" t="s">
         <v>1945</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="E100" s="2" t="s">
         <v>1946</v>
       </c>
-      <c r="E100" s="2" t="s">
+      <c r="F100" s="2" t="s">
         <v>1947</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="G100" s="2" t="s">
         <v>1948</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>1949</v>
       </c>
     </row>
     <row r="101" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="2" t="s">
+        <v>1949</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>1810</v>
+      </c>
+      <c r="D101" s="2" t="s">
         <v>1950</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>1811</v>
-      </c>
-      <c r="D101" s="2" t="s">
+      <c r="E101" s="2" t="s">
         <v>1951</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="F101" s="2" t="s">
         <v>1952</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="G101" s="2" t="s">
         <v>1953</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>1954</v>
       </c>
     </row>
     <row r="102" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -15383,124 +15383,124 @@
         <v>50</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="D102" s="2" t="s">
+        <v>1954</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>1955</v>
       </c>
-      <c r="E102" s="2" t="s">
+      <c r="F102" s="2" t="s">
         <v>1956</v>
       </c>
-      <c r="F102" s="2" t="s">
+      <c r="G102" s="2" t="s">
         <v>1957</v>
-      </c>
-      <c r="G102" s="2" t="s">
-        <v>1958</v>
       </c>
     </row>
     <row r="103" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>1959</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>1960</v>
       </c>
-      <c r="D103" s="2" t="s">
+      <c r="E103" s="2" t="s">
         <v>1961</v>
       </c>
-      <c r="E103" s="2" t="s">
+      <c r="F103" s="2" t="s">
         <v>1962</v>
       </c>
-      <c r="F103" s="2" t="s">
+      <c r="G103" s="2" t="s">
         <v>1963</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>1964</v>
       </c>
     </row>
     <row r="104" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="2" t="s">
+        <v>1964</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>1965</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="D104" s="2" t="s">
+        <v>1965</v>
+      </c>
+      <c r="E104" s="2" t="s">
         <v>1966</v>
       </c>
-      <c r="D104" s="2" t="s">
-        <v>1966</v>
-      </c>
-      <c r="E104" s="2" t="s">
+      <c r="F104" s="2" t="s">
         <v>1967</v>
       </c>
-      <c r="F104" s="2" t="s">
+      <c r="G104" s="2" t="s">
         <v>1968</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>1969</v>
       </c>
     </row>
     <row r="105" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="2" t="s">
+        <v>1969</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>1970</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="D105" s="2" t="s">
         <v>1971</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="E105" s="2" t="s">
         <v>1972</v>
       </c>
-      <c r="E105" s="2" t="s">
+      <c r="F105" s="2" t="s">
         <v>1973</v>
       </c>
-      <c r="F105" s="2" t="s">
+      <c r="G105" s="2" t="s">
         <v>1974</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>1975</v>
       </c>
     </row>
     <row r="106" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="2" t="s">
+        <v>1975</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>1976</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="D106" s="2" t="s">
         <v>1977</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="E106" s="2" t="s">
         <v>1978</v>
       </c>
-      <c r="E106" s="2" t="s">
+      <c r="F106" s="2" t="s">
         <v>1979</v>
       </c>
-      <c r="F106" s="2" t="s">
+      <c r="G106" s="2" t="s">
         <v>1980</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>1981</v>
       </c>
     </row>
     <row r="107" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B107" s="2" t="s">
+        <v>1981</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>1982</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="D107" s="2" t="s">
         <v>1983</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="E107" s="2" t="s">
         <v>1984</v>
       </c>
-      <c r="E107" s="2" t="s">
+      <c r="F107" s="2" t="s">
         <v>1985</v>
       </c>
-      <c r="F107" s="2" t="s">
+      <c r="G107" s="2" t="s">
         <v>1986</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>1987</v>
       </c>
     </row>
     <row r="111" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B111" s="3" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.2">
@@ -15525,22 +15525,22 @@
     </row>
     <row r="114" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B114" s="7" t="s">
+        <v>2038</v>
+      </c>
+      <c r="C114" s="7" t="s">
         <v>2039</v>
       </c>
-      <c r="C114" s="7" t="s">
+      <c r="D114" s="7" t="s">
+        <v>2043</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>2042</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>2041</v>
+      </c>
+      <c r="G114" s="7" t="s">
         <v>2040</v>
-      </c>
-      <c r="D114" s="7" t="s">
-        <v>2044</v>
-      </c>
-      <c r="E114" s="7" t="s">
-        <v>2043</v>
-      </c>
-      <c r="F114" s="7" t="s">
-        <v>2042</v>
-      </c>
-      <c r="G114" s="7" t="s">
-        <v>2041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>